<commit_message>
sua yeu cau cong viec
</commit_message>
<xml_diff>
--- a/QLQuanCaPhe/Nội dung + thành viên/Công việc cần làm.xlsx
+++ b/QLQuanCaPhe/Nội dung + thành viên/Công việc cần làm.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Trình lập kế hoạch Dự án</t>
   </si>
@@ -208,10 +208,22 @@
     <t>Thống kê bán hàng(món bán chạy hay chậm)</t>
   </si>
   <si>
+    <t>Thống kê app bán hàng</t>
+  </si>
+  <si>
     <t>Thiết kế database</t>
   </si>
   <si>
-    <t>Thiết kế giao diện</t>
+    <t>Thiết kế giao diện ( Mockup)</t>
+  </si>
+  <si>
+    <t>Làm bảng yêu cầu và trách nhiệm</t>
+  </si>
+  <si>
+    <t>Làm các Daigrams</t>
+  </si>
+  <si>
+    <t>Làm thiết kế giao diện</t>
   </si>
 </sst>
 </file>
@@ -219,10 +231,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_-* #,##0\ &quot;₫&quot;_-;\-* #,##0\ &quot;₫&quot;_-;_-* &quot;-&quot;\ &quot;₫&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0\ &quot;₫&quot;_-;\-* #,##0\ &quot;₫&quot;_-;_-* &quot;-&quot;\ &quot;₫&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -324,14 +336,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -340,6 +344,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -353,13 +365,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -376,6 +381,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -383,9 +396,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -463,175 +475,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -714,21 +726,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -743,13 +740,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -769,17 +770,28 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -797,30 +809,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyFill="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -834,12 +846,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyFill="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="1" fontId="6" fillId="2" borderId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -847,52 +859,52 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="3" applyFill="0" applyProtection="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="3" applyFill="0" applyProtection="0">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -921,7 +933,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="18">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="59">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="60">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="2" borderId="1" xfId="28">
@@ -945,7 +957,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="20" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="3" xfId="57">
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="3" xfId="56">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="33" applyFont="1">
@@ -960,10 +972,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="58" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="60" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="59" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="60" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="59" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="13" applyAlignment="1">
@@ -984,16 +996,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="40" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="60" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="59" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="60" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="59" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="51" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="56" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="57" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1054,11 +1066,11 @@
     <cellStyle name="Accent6" xfId="53" builtinId="49"/>
     <cellStyle name="40% - Accent6" xfId="54" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="55" builtinId="52"/>
-    <cellStyle name="% hoàn thành (ngoài kế hoạch) chú giải" xfId="56"/>
-    <cellStyle name="Đầu đề Thời gian" xfId="57"/>
+    <cellStyle name="Đầu đề Thời gian" xfId="56"/>
+    <cellStyle name="% hoàn thành (ngoài kế hoạch) chú giải" xfId="57"/>
     <cellStyle name="Chú giải kế hoạch" xfId="58"/>
-    <cellStyle name="Điều khiển Tô sáng Thời gian" xfId="59"/>
-    <cellStyle name="Nhãn" xfId="60"/>
+    <cellStyle name="Nhãn" xfId="59"/>
+    <cellStyle name="Điều khiển Tô sáng Thời gian" xfId="60"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -1430,10 +1442,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BO27"/>
+  <dimension ref="B1:BO33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1"/>
@@ -1767,13 +1779,13 @@
         <v>10</v>
       </c>
       <c r="E5" s="18">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F5" s="18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G5" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="2:7">
@@ -1787,13 +1799,13 @@
         <v>10</v>
       </c>
       <c r="E6" s="18">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F6" s="18">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G6" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="2:7">
@@ -1807,13 +1819,13 @@
         <v>10</v>
       </c>
       <c r="E7" s="18">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F7" s="18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G7" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="2:7">
@@ -1827,13 +1839,13 @@
         <v>10</v>
       </c>
       <c r="E8" s="18">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F8" s="18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G8" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="2:7">
@@ -1847,13 +1859,13 @@
         <v>15</v>
       </c>
       <c r="E9" s="18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F9" s="18">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G9" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="2:7">
@@ -1867,13 +1879,13 @@
         <v>10</v>
       </c>
       <c r="E10" s="18">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F10" s="18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G10" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="2:7">
@@ -1887,13 +1899,13 @@
         <v>20</v>
       </c>
       <c r="E11" s="18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F11" s="18">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G11" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="2:7">
@@ -1913,7 +1925,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="2:7">
@@ -1933,7 +1945,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" customHeight="1" spans="2:7">
@@ -1953,7 +1965,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" customHeight="1" spans="2:7">
@@ -1973,7 +1985,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" customHeight="1" spans="2:7">
@@ -1993,7 +2005,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" customHeight="1" spans="2:7">
@@ -2013,7 +2025,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" customHeight="1" spans="2:7">
@@ -2033,7 +2045,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" customHeight="1" spans="2:7">
@@ -2053,7 +2065,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" customHeight="1" spans="2:7">
@@ -2073,7 +2085,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" customHeight="1" spans="2:7">
@@ -2093,7 +2105,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="2:7">
@@ -2113,7 +2125,7 @@
         <v>0</v>
       </c>
       <c r="G22" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" customHeight="1" spans="2:7">
@@ -2133,7 +2145,7 @@
         <v>0</v>
       </c>
       <c r="G23" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" customHeight="1" spans="2:7">
@@ -2153,7 +2165,7 @@
         <v>0</v>
       </c>
       <c r="G24" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" customHeight="1" spans="2:7">
@@ -2173,7 +2185,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" customHeight="1" spans="2:7">
@@ -2181,10 +2193,10 @@
         <v>36</v>
       </c>
       <c r="C26" s="18">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D26" s="18">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E26" s="18">
         <v>0</v>
@@ -2193,7 +2205,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" customHeight="1" spans="2:7">
@@ -2213,8 +2225,104 @@
         <v>0</v>
       </c>
       <c r="G27" s="19">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" customHeight="1" spans="2:7">
+      <c r="B28" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="18">
+        <v>1</v>
+      </c>
+      <c r="D28" s="18">
+        <v>5</v>
+      </c>
+      <c r="E28" s="18">
+        <v>0</v>
+      </c>
+      <c r="F28" s="18">
+        <v>0</v>
+      </c>
+      <c r="G28" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" customHeight="1" spans="2:7">
+      <c r="B29" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="18">
+        <v>10</v>
+      </c>
+      <c r="D29" s="18">
+        <v>7</v>
+      </c>
+      <c r="E29" s="18">
+        <v>12</v>
+      </c>
+      <c r="F29" s="18">
+        <v>17</v>
+      </c>
+      <c r="G29" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customHeight="1" spans="2:7">
+      <c r="B30" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="18">
+        <v>24</v>
+      </c>
+      <c r="D30" s="18">
+        <v>7</v>
+      </c>
+      <c r="E30" s="18">
+        <v>24</v>
+      </c>
+      <c r="F30" s="18">
+        <v>20</v>
+      </c>
+      <c r="G30" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" customHeight="1" spans="2:7">
+      <c r="B31" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="18">
+        <v>30</v>
+      </c>
+      <c r="D31" s="18">
+        <v>7</v>
+      </c>
+      <c r="E31" s="18">
+        <v>30</v>
+      </c>
+      <c r="F31" s="18">
+        <v>37</v>
+      </c>
+      <c r="G31" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" customHeight="1" spans="2:7">
+      <c r="B32" s="17"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="19"/>
+    </row>
+    <row r="33" customHeight="1" spans="2:7">
+      <c r="B33" s="17"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -2237,12 +2345,12 @@
       <formula>H$4=thời_gian_được_chọn</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B28:BO28">
+  <conditionalFormatting sqref="B34:BO34">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:BO27">
+  <conditionalFormatting sqref="H5:BO33">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>Phần_trăm_Hoàn_thành</formula>
     </cfRule>
@@ -2270,10 +2378,10 @@
   </conditionalFormatting>
   <dataValidations count="16">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Ô chú giải này cho biết thời lượng thực tế" sqref="S2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trình lập kế hoạch dự án sử dụng thời gian cho các khoảng thời gian. Bắt đầu=1 là thời gian 1 và thời lượng=5 là dự án có 5 giai đoạn bắt đầu từ thời gian bắt đầu. Nhập dữ liệu bắt đầu vào B5 để cập nhật biểu đồ" sqref="A1"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Nhập giá trị từ 1 đến 60 hoặc chọn thời gian từ danh sách - nhấn HỦY BỎ, ALT+MŨI TÊN XUỐNG, rồi nhấn ENTER để chọn giá trị" prompt="Nhập thời gian trong phạm vi từ 1 đến 60 hoặc chọn một thời gian từ danh sách. Nhấn ALT+MŨI TÊN XUỐNG để dẫn hướng trong danh sách, rồi nhấn ENTER để chọn giá trị" sqref="H2" errorStyle="warning">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Trình lập kế hoạch dự án sử dụng thời gian cho các khoảng thời gian. Bắt đầu=1 là thời gian 1 và thời lượng=5 là dự án có 5 giai đoạn bắt đầu từ thời gian bắt đầu. Nhập dữ liệu bắt đầu vào B5 để cập nhật biểu đồ" sqref="A1"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Tiêu đề của dự án. Nhập tiêu đề mới vào ô này. Tô sáng thời gian trong H2. Chú thích biểu đồ nằm trong J2 đến AI2" sqref="B1"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Chọn thời gian để tô sáng ở H2. Chú giải biểu đồ nằm trong J2 đến AI2" sqref="B2:F2"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Ô chú giải này cho biết thời lượng kế hoạch" sqref="J2"/>

</xml_diff>